<commit_message>
Update dealer and customer password files and change database password
</commit_message>
<xml_diff>
--- a/passwords/customers_password.xlsx
+++ b/passwords/customers_password.xlsx
@@ -462,7 +462,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$2b$10$eO6XzDdeaw6FRFeEj3FIC.ZP.lTrinSO.6lxiCHuX5JjNgSEmoz..</t>
+          <t>$2b$10$sZ9I.kZKPGy.I/KTpI5T8.AFs/is1186iazck4NjzqaAaUGdCXUeS</t>
         </is>
       </c>
     </row>
@@ -479,7 +479,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$2b$10$hZvYGau0pDstfH.Rj4fUbe/KhTumfR6OoPo9dKNCoD.7GmRcehu52</t>
+          <t>$2b$10$0SehfwimNn99Ry4wx67EK.BlEEUTvXK0towkfF7pBlJj/rliymALy</t>
         </is>
       </c>
     </row>
@@ -496,7 +496,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>$2b$10$9xtOTS009md8VIfeXq61Qup5BywUYzOeeJXXKgZcojuF3HrATzqSa</t>
+          <t>$2b$10$oPS4zDbAsMk34rnjfQwZleN/isd91acC58FW3vYrHidfQbTukNmlG</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>$2b$10$GzWHM1m77lD8ZQS3kISMx.Cds8lG8V0f0JA05y29XjMangpy71BPW</t>
+          <t>$2b$10$/cFPBjkc3UetzO3KUP03S..MMVjjEz2Rm6Yqre/l/PK4El.8J6JHC</t>
         </is>
       </c>
     </row>
@@ -530,7 +530,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>$2b$10$PVKdNJasAuJi69BqBVbqJedpEgHJFWeeN9Iju3D/j/ePwkpFta0BS</t>
+          <t>$2b$10$55ByGzitYQHrru.8AnjSxuw1zPS.C27RtM5hbFJNLsT09VuuofIke</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$2b$10$dHc/vtyLnkPWy1GL69rRBOlImAdihiV6H7f34lhuQvUqOSq.2Q5p6</t>
+          <t>$2b$10$YPXcA20ejcwBpKg1gfGEeuXwrRIyKF9X4eyydkI6ZU57/Y2mZALOO</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>$2b$10$dwySoHFtLCqGx5cZcmW.WOslWzJcLn/FScneQhxgNBkkG5ir90q4m</t>
+          <t>$2b$10$irTvl2EQ6wlG2Wv9AYKb5uuOaQAs5W8rwcQFXUZnRfUWZ9xWCufLW</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>$2b$10$N1Pp3OZtkWYTSt3DXeoq0uiQny5pcu7yLx4EMTJXckWlyP8uF4/7y</t>
+          <t>$2b$10$5RBb8wiTN.smh8Ku3QzVqea.7drhdd080CNVY.NOMhQYoJVb90Epm</t>
         </is>
       </c>
     </row>
@@ -598,7 +598,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>$2b$10$M4eVhiBTtrwdVAihPQUUz.O6fkANZf1FWcv5gmGiO5dIXij7LIpf2</t>
+          <t>$2b$10$VRy8CdwHSIsV6kfG969ujOG9fk/Se2kYp1FhpKp1z1va3s9GaJG7S</t>
         </is>
       </c>
     </row>
@@ -615,7 +615,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>$2b$10$.1NMGuAIhlfAOLIEjBfxC.FoPeKdhcKhmysEsosLq.bO6MbZHCvTi</t>
+          <t>$2b$10$NX6o9XKLPoYAvXlmDLeq2eZnSSZkn0yuA2ULjldKqExNQByELkBwq</t>
         </is>
       </c>
     </row>
@@ -632,7 +632,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>$2b$10$ScbevcukV9aFiwfaCcN2CuolbFGkkwDeCOCYdJJrmTGxb14D8n2DW</t>
+          <t>$2b$10$ZboSh6qZG1IyjobcD/3J3u6ummjcLGudjSkagbTyDVqsLpzb0MP7K</t>
         </is>
       </c>
     </row>
@@ -649,7 +649,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>$2b$10$D.lJWaQ1R8Bf0.HCgz943.XmsWP24IX7FNqdOkKHj8.yWD3B6igmG</t>
+          <t>$2b$10$evUKf4g0HIZuN.SqFf7UDOscnmvJn7OXZvaYqn3E1xp5fuI6RcL4G</t>
         </is>
       </c>
     </row>
@@ -666,7 +666,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>$2b$10$JxVPLlLbo67E07g4Zk2D2OFhZHareOXkwm8eZFb.ZvLrlp7RZQR7i</t>
+          <t>$2b$10$s6m3iyrtGhn4y/pTinLNjutieRHaMtrdDpuHeb2W0jE4cXo0oj6dG</t>
         </is>
       </c>
     </row>
@@ -683,7 +683,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>$2b$10$pTdjajKHoLReLBdyVyZ6BukL2Vq8Cz5Rbh.Q3YYibyqnULOz1DtqS</t>
+          <t>$2b$10$hxRCnhKBOwFlO/FWrzzYrOQPxzVuNwSe84BZnqataGbt0InoaRht2</t>
         </is>
       </c>
     </row>
@@ -700,7 +700,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>$2b$10$BduR986KaBOYLlHpsIlXWOxh.HFktqF.gJRV2jFAzGCj9LiQgd1dq</t>
+          <t>$2b$10$s8/pAqjiL7kd2I8rJxaagu49gW8aFcCvoD99ICZpVMal/mEe8v/B2</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>$2b$10$5kJpNfj58vhPUm9pH9VKsu/8XNkTDGAOEGC9DJ151Et338ID8d88q</t>
+          <t>$2b$10$TaeCGp5/4Jr0SncOiyRCQuoAKIxZ/Xo2cIEE33vPCYjniDF.uZTB.</t>
         </is>
       </c>
     </row>
@@ -734,7 +734,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>$2b$10$39EOsVOP5s.oJgIe3aIM.e1xuxx1Nfvb4nbPF2ibZTowDs8dwP.AS</t>
+          <t>$2b$10$qVeeMSW3qJKFvC5ziAON0OpkaiadsvBpounkzyRxluJFHxFB83dma</t>
         </is>
       </c>
     </row>
@@ -751,7 +751,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>$2b$10$9LUjSODJRwCrjAsKlVao5eCPhUi6e6sY7OC8gncd2gou91TJ88b8y</t>
+          <t>$2b$10$6tQmAirHV92YMV5Jm17reuxAOr05zWh5ZgWDRn1K2B4X24J9ZmRM2</t>
         </is>
       </c>
     </row>
@@ -768,7 +768,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>$2b$10$d.L0TYmDGYPuzbAutkfDJeJn64XQS0BVI/bfrBNiOPBr6p1Pb7N.W</t>
+          <t>$2b$10$yKx2pp5hQRlyBObOjXcnJejHKH97Mt8p6rhffc9H7YkIL72X9dZCG</t>
         </is>
       </c>
     </row>
@@ -785,7 +785,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>$2b$10$sxwcBxOat/5.ns5ndVFNsueI8otG1SgAWNhi/stZybCuSezfsjfWK</t>
+          <t>$2b$10$8ZCe3Ej86mFfvnvQxrWqO.U2O7eV5lrsBn4VLiG6nzkhQt16b4FMy</t>
         </is>
       </c>
     </row>
@@ -802,7 +802,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>$2b$10$yKofqAfyYuWuJZzo3Q6fbu53.ydAAgXI69L4MHIJPNNJGC9/WWOya</t>
+          <t>$2b$10$F4MBFxVvQDHfcp6ZAE86..3URH5ndxU/VVTbU3QsKLk6NbF.uvzg2</t>
         </is>
       </c>
     </row>
@@ -819,7 +819,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>$2b$10$L4NMv2r5Se5tbLh8HJ/iWurvB2QPXePzfylOTLaeV1Y2eee./AoIy</t>
+          <t>$2b$10$rM/s0OpdpcidLJGhyYRnMermYbrXaN.wGcZ3IsLugD2UMoDPS/Wcu</t>
         </is>
       </c>
     </row>
@@ -836,7 +836,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>$2b$10$LvqFlptUgtAtDgzPNDNjWebp7yE/J3X7n7oHmNuBpJ7wHunWFaOwq</t>
+          <t>$2b$10$.2QCHEDqcPFJ/CgT5t7LcO9gge657lH.Vk4BEbxbI1.BtE3EIimrm</t>
         </is>
       </c>
     </row>
@@ -853,7 +853,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>$2b$10$C0RO.9JexkJxxql5vAV2tuaZtyJAqBfmIhc6F6/AE9mZ0SEOqkQ6G</t>
+          <t>$2b$10$p50hTk3v2cPELVAW3kDw2OgyEol6y6EPYUlHmJ6qEScwXIHkN35/u</t>
         </is>
       </c>
     </row>
@@ -870,7 +870,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>$2b$10$Q1L71PpouINSUzYCrCCpoeIUX1ngHj7fG/v4sFpNCPhL19rRxxAfO</t>
+          <t>$2b$10$VdDRL..NFjg1jRvxVcbokOBSPpn2lyRU7KiJ0lNJyGAXfOeOYvdbK</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update dealer and customer password files
</commit_message>
<xml_diff>
--- a/passwords/customers_password.xlsx
+++ b/passwords/customers_password.xlsx
@@ -462,7 +462,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$2b$10$sZ9I.kZKPGy.I/KTpI5T8.AFs/is1186iazck4NjzqaAaUGdCXUeS</t>
+          <t>$2b$10$g3pe90i7yVrJneH90WOn.O1FZCPS./1aXwd.2d1RsB1eIHGHIlOLG</t>
         </is>
       </c>
     </row>
@@ -479,7 +479,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$2b$10$0SehfwimNn99Ry4wx67EK.BlEEUTvXK0towkfF7pBlJj/rliymALy</t>
+          <t>$2b$10$mT/5RgxVZypYOBaRKina6OTK9NsyjZLJK8mHjMo26yhKiDayAwAqi</t>
         </is>
       </c>
     </row>
@@ -496,7 +496,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>$2b$10$oPS4zDbAsMk34rnjfQwZleN/isd91acC58FW3vYrHidfQbTukNmlG</t>
+          <t>$2b$10$pMZqe8RF7Y4H4tG7rY6Tf.5VQGIPyAEM.ooqE6CecRknahO.Za3SC</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>$2b$10$/cFPBjkc3UetzO3KUP03S..MMVjjEz2Rm6Yqre/l/PK4El.8J6JHC</t>
+          <t>$2b$10$XrDka72pDjPMXX6NEXx6a.uhr/5SQ1r/pyN5omWvUTM7GJENM7VAG</t>
         </is>
       </c>
     </row>
@@ -530,7 +530,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>$2b$10$55ByGzitYQHrru.8AnjSxuw1zPS.C27RtM5hbFJNLsT09VuuofIke</t>
+          <t>$2b$10$eUwCZTqheO0Vqp6C6P2LJuV7n4tc0UbkRvD04DQZjYJRZESbGcAQ6</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$2b$10$YPXcA20ejcwBpKg1gfGEeuXwrRIyKF9X4eyydkI6ZU57/Y2mZALOO</t>
+          <t>$2b$10$vL8q2ZHPIGcqDczHXaz4YOrqF7ZLxKCQ6JreHjd7zB9yuUcqKVQSq</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>$2b$10$irTvl2EQ6wlG2Wv9AYKb5uuOaQAs5W8rwcQFXUZnRfUWZ9xWCufLW</t>
+          <t>$2b$10$5z34zPmPRdZPGUkRxSW/KOybRVrmp6Zj1LsSUaPiMFyaHCIXTvUom</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>$2b$10$5RBb8wiTN.smh8Ku3QzVqea.7drhdd080CNVY.NOMhQYoJVb90Epm</t>
+          <t>$2b$10$NrTJqztu/UtsqPQsKdBfWuGMNlPuCZssYMYHLlsjbWlBdlzIlVIRm</t>
         </is>
       </c>
     </row>
@@ -598,7 +598,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>$2b$10$VRy8CdwHSIsV6kfG969ujOG9fk/Se2kYp1FhpKp1z1va3s9GaJG7S</t>
+          <t>$2b$10$PKZGj4UrNjYU9hwj7oGOF.QpayoBANS3kxp9YSdLkMnBoK8b.s2O2</t>
         </is>
       </c>
     </row>
@@ -615,7 +615,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>$2b$10$NX6o9XKLPoYAvXlmDLeq2eZnSSZkn0yuA2ULjldKqExNQByELkBwq</t>
+          <t>$2b$10$HoEU.ZazQNoZOf0n98m2A.7nDIO9bAFu9cU3kxwhJy5CNw87ml1rG</t>
         </is>
       </c>
     </row>
@@ -632,7 +632,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>$2b$10$ZboSh6qZG1IyjobcD/3J3u6ummjcLGudjSkagbTyDVqsLpzb0MP7K</t>
+          <t>$2b$10$9ALv.H2NmoWaXzWT6F5vJuieLbnuSyKESdH8RQegNDv.v/qn1xpWu</t>
         </is>
       </c>
     </row>
@@ -649,7 +649,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>$2b$10$evUKf4g0HIZuN.SqFf7UDOscnmvJn7OXZvaYqn3E1xp5fuI6RcL4G</t>
+          <t>$2b$10$sBPE0PFJPs4eTDa4ckta0OaOc62wrcfKmQAxyc30WTyVllDCNrhcm</t>
         </is>
       </c>
     </row>
@@ -666,7 +666,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>$2b$10$s6m3iyrtGhn4y/pTinLNjutieRHaMtrdDpuHeb2W0jE4cXo0oj6dG</t>
+          <t>$2b$10$JRkzFvSLfKI5hJ3EknyV7.o./Qa8DwkeuOqCTTtGo4UBPgTdK0X06</t>
         </is>
       </c>
     </row>
@@ -683,7 +683,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>$2b$10$hxRCnhKBOwFlO/FWrzzYrOQPxzVuNwSe84BZnqataGbt0InoaRht2</t>
+          <t>$2b$10$OAGgl7pREzHxi33EVzMKe.tatRR/eMKEHFEDFH.FHdx3HZZrjZ6fO</t>
         </is>
       </c>
     </row>
@@ -700,7 +700,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>$2b$10$s8/pAqjiL7kd2I8rJxaagu49gW8aFcCvoD99ICZpVMal/mEe8v/B2</t>
+          <t>$2b$10$Vk658euGqnyNZj/80SXOleuICWZZo1JX1QOVwICr6HI46VCydtLmG</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>$2b$10$TaeCGp5/4Jr0SncOiyRCQuoAKIxZ/Xo2cIEE33vPCYjniDF.uZTB.</t>
+          <t>$2b$10$okyuJCgeUS/zUqL1lDGJvOjeGMQ6Q1D.zak4rzO7Yrdjddqi87Nru</t>
         </is>
       </c>
     </row>
@@ -734,7 +734,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>$2b$10$qVeeMSW3qJKFvC5ziAON0OpkaiadsvBpounkzyRxluJFHxFB83dma</t>
+          <t>$2b$10$mGs65vl5pjU0gjzTnbVC9u21.yOagrsB0p8BCYkg83ACNK397tpga</t>
         </is>
       </c>
     </row>
@@ -751,7 +751,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>$2b$10$6tQmAirHV92YMV5Jm17reuxAOr05zWh5ZgWDRn1K2B4X24J9ZmRM2</t>
+          <t>$2b$10$TwzC955E72vyJx0VCyYgG.WcIfEgqq22xcAkAQOsrF4IwVuR5SAvy</t>
         </is>
       </c>
     </row>
@@ -768,7 +768,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>$2b$10$yKx2pp5hQRlyBObOjXcnJejHKH97Mt8p6rhffc9H7YkIL72X9dZCG</t>
+          <t>$2b$10$ViBzSWs9pVaKGPSbYBkOZOQRjd5m758q7YJ0U9fgbE/W3i59k1SyW</t>
         </is>
       </c>
     </row>
@@ -785,7 +785,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>$2b$10$8ZCe3Ej86mFfvnvQxrWqO.U2O7eV5lrsBn4VLiG6nzkhQt16b4FMy</t>
+          <t>$2b$10$zbQos.imaLJhVepjErMaAerC99GUxFxOV2r34wjhpuOEEIGVahO0i</t>
         </is>
       </c>
     </row>
@@ -802,7 +802,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>$2b$10$F4MBFxVvQDHfcp6ZAE86..3URH5ndxU/VVTbU3QsKLk6NbF.uvzg2</t>
+          <t>$2b$10$Fd1XSabXEwjiJNLocx6/J.gwwUC.I3RFgmMSnm8QZVB2kCvvX9DMS</t>
         </is>
       </c>
     </row>
@@ -819,7 +819,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>$2b$10$rM/s0OpdpcidLJGhyYRnMermYbrXaN.wGcZ3IsLugD2UMoDPS/Wcu</t>
+          <t>$2b$10$nT5N8YyDvyfF6jBqdMrASeOppYMXTiDavONk6koDR.0prmDow3Zx2</t>
         </is>
       </c>
     </row>
@@ -836,7 +836,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>$2b$10$.2QCHEDqcPFJ/CgT5t7LcO9gge657lH.Vk4BEbxbI1.BtE3EIimrm</t>
+          <t>$2b$10$HwahCWjiPns4h6MkeohBe.YQmvy7o66K/IeLlvIeiSPM5hr1zrmWq</t>
         </is>
       </c>
     </row>
@@ -853,7 +853,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>$2b$10$p50hTk3v2cPELVAW3kDw2OgyEol6y6EPYUlHmJ6qEScwXIHkN35/u</t>
+          <t>$2b$10$UoiN1Gw07cn.16oD7YIww.qXM7HUrvegCndaNkNk5SuRGc0nQOHAS</t>
         </is>
       </c>
     </row>
@@ -870,7 +870,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>$2b$10$VdDRL..NFjg1jRvxVcbokOBSPpn2lyRU7KiJ0lNJyGAXfOeOYvdbK</t>
+          <t>$2b$10$JC9UU0nbTprkUJzlsgezf.V6knLGVWkSxevXt8CK3IwyLVbnTFmme</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update password files and database configuration
</commit_message>
<xml_diff>
--- a/passwords/customers_password.xlsx
+++ b/passwords/customers_password.xlsx
@@ -462,7 +462,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$2b$10$sZ9I.kZKPGy.I/KTpI5T8.AFs/is1186iazck4NjzqaAaUGdCXUeS</t>
+          <t>$2b$10$ZEaFnEVEQI38wULA.FIu0.tKDH0jKtVtzuYpnhB178wasn.wIB35.</t>
         </is>
       </c>
     </row>
@@ -479,7 +479,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$2b$10$0SehfwimNn99Ry4wx67EK.BlEEUTvXK0towkfF7pBlJj/rliymALy</t>
+          <t>$2b$10$lmMyT4ygt.yM9AwW6svphOib69jMRlrFbzmLcHr/DpM1NBSBfdu2W</t>
         </is>
       </c>
     </row>
@@ -496,7 +496,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>$2b$10$oPS4zDbAsMk34rnjfQwZleN/isd91acC58FW3vYrHidfQbTukNmlG</t>
+          <t>$2b$10$JcBFILFDaQ6/8l7fNMe.j.t0TUNP8o2.SZUlNDMnRIAmRVV6oLWda</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>$2b$10$/cFPBjkc3UetzO3KUP03S..MMVjjEz2Rm6Yqre/l/PK4El.8J6JHC</t>
+          <t>$2b$10$EgE8ymvINud3RmuzK1gqZ.Dzn.VEVgJXTa23bqwKfA64bcZGllnfi</t>
         </is>
       </c>
     </row>
@@ -530,7 +530,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>$2b$10$55ByGzitYQHrru.8AnjSxuw1zPS.C27RtM5hbFJNLsT09VuuofIke</t>
+          <t>$2b$10$7Lty84joZ8e9arEUQJZzLeJvyJql.b1P.PgikPyLI.rbrJ6yOPIxG</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$2b$10$YPXcA20ejcwBpKg1gfGEeuXwrRIyKF9X4eyydkI6ZU57/Y2mZALOO</t>
+          <t>$2b$10$jMTy.aT1lp68nw/5k3Nch.4eM0duCoE68HkW.IvA6/njcS/E4djia</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>$2b$10$irTvl2EQ6wlG2Wv9AYKb5uuOaQAs5W8rwcQFXUZnRfUWZ9xWCufLW</t>
+          <t>$2b$10$o2NeTYIOOF4AuJsGONOIrOWLqQnQX5nmWiiiFeTK8aAfimHuzfGmy</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>$2b$10$5RBb8wiTN.smh8Ku3QzVqea.7drhdd080CNVY.NOMhQYoJVb90Epm</t>
+          <t>$2b$10$.Mw.eubcNkG9kwUg6F4Ttu0m1.vSv268YJP44TdRXoIic2IOrNjmG</t>
         </is>
       </c>
     </row>
@@ -598,7 +598,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>$2b$10$VRy8CdwHSIsV6kfG969ujOG9fk/Se2kYp1FhpKp1z1va3s9GaJG7S</t>
+          <t>$2b$10$TdeIp9uu2CfuPU.EU8z.RenHpTr3y6xgBhorjX/dvaEDE/q/zurB6</t>
         </is>
       </c>
     </row>
@@ -615,7 +615,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>$2b$10$NX6o9XKLPoYAvXlmDLeq2eZnSSZkn0yuA2ULjldKqExNQByELkBwq</t>
+          <t>$2b$10$bf5yzmJe7TvW3C2dNm0SHuJtBjS/f8x7Ll3PsL.Qsv9taTynTM4j.</t>
         </is>
       </c>
     </row>
@@ -632,7 +632,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>$2b$10$ZboSh6qZG1IyjobcD/3J3u6ummjcLGudjSkagbTyDVqsLpzb0MP7K</t>
+          <t>$2b$10$5i2P7Qvf9Xmq8jb8d5wMceTY3QBgH346HyMFGu5dIzXRLAr6o2FlS</t>
         </is>
       </c>
     </row>
@@ -649,7 +649,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>$2b$10$evUKf4g0HIZuN.SqFf7UDOscnmvJn7OXZvaYqn3E1xp5fuI6RcL4G</t>
+          <t>$2b$10$YUGe5U.T0V8JeIbcXjB6Ye.USepVA.U6yxr6qKuOBgFKvT/rwjg66</t>
         </is>
       </c>
     </row>
@@ -666,7 +666,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>$2b$10$s6m3iyrtGhn4y/pTinLNjutieRHaMtrdDpuHeb2W0jE4cXo0oj6dG</t>
+          <t>$2b$10$T8kw/A8J4tv/Y9sYQlHZi.wPqngiOtfC4D2WtA9jvqUauuOaBC.4y</t>
         </is>
       </c>
     </row>
@@ -683,7 +683,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>$2b$10$hxRCnhKBOwFlO/FWrzzYrOQPxzVuNwSe84BZnqataGbt0InoaRht2</t>
+          <t>$2b$10$.OBbHlvnwMqwuIwi.gDZGeRgpDgDCu5Xd9BeFhrYS0dDvILXHNMJy</t>
         </is>
       </c>
     </row>
@@ -700,7 +700,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>$2b$10$s8/pAqjiL7kd2I8rJxaagu49gW8aFcCvoD99ICZpVMal/mEe8v/B2</t>
+          <t>$2b$10$x/KT0f.ERbvz94sFnA1tZuX/HHFFvPUCjZrXDvLL8asl175Umb8MS</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>$2b$10$TaeCGp5/4Jr0SncOiyRCQuoAKIxZ/Xo2cIEE33vPCYjniDF.uZTB.</t>
+          <t>$2b$10$gkgY0Va7ioozVHwAkB3AjOGV3AsZTGLZXr13EyKd7JNdI8qr16/3u</t>
         </is>
       </c>
     </row>
@@ -734,7 +734,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>$2b$10$qVeeMSW3qJKFvC5ziAON0OpkaiadsvBpounkzyRxluJFHxFB83dma</t>
+          <t>$2b$10$vWUVCX6OIm1xvqYhEgSsf.CZpecmdSivvSUQQKxwDNlNc431PQku2</t>
         </is>
       </c>
     </row>
@@ -751,7 +751,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>$2b$10$6tQmAirHV92YMV5Jm17reuxAOr05zWh5ZgWDRn1K2B4X24J9ZmRM2</t>
+          <t>$2b$10$S5lAV2nohy6k5pV8jsnq5Ou08z.IXiRZPyk6DG.X6SAsVS2WcHBvO</t>
         </is>
       </c>
     </row>
@@ -768,7 +768,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>$2b$10$yKx2pp5hQRlyBObOjXcnJejHKH97Mt8p6rhffc9H7YkIL72X9dZCG</t>
+          <t>$2b$10$5QMDkzJaq1OIbAUduJyUa.tfCM49y527yikoAXNJI5hJEUrZSIyKi</t>
         </is>
       </c>
     </row>
@@ -785,7 +785,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>$2b$10$8ZCe3Ej86mFfvnvQxrWqO.U2O7eV5lrsBn4VLiG6nzkhQt16b4FMy</t>
+          <t>$2b$10$mn8VBWmeIxbrvJpPvW9jjexm1ZHT1T6Rae.uiIeA.2jiETBHHsFgC</t>
         </is>
       </c>
     </row>
@@ -802,7 +802,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>$2b$10$F4MBFxVvQDHfcp6ZAE86..3URH5ndxU/VVTbU3QsKLk6NbF.uvzg2</t>
+          <t>$2b$10$CMa3HfVaanJXM/RZ0z68Ku.Zgl26os6idVi0aeN0/od/9iZAK1XmG</t>
         </is>
       </c>
     </row>
@@ -819,7 +819,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>$2b$10$rM/s0OpdpcidLJGhyYRnMermYbrXaN.wGcZ3IsLugD2UMoDPS/Wcu</t>
+          <t>$2b$10$g.ZsLVVjqH1M0y8Dfv.1s.gFEOG1oidNCgyULohKMn0HFIK1OCING</t>
         </is>
       </c>
     </row>
@@ -836,7 +836,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>$2b$10$.2QCHEDqcPFJ/CgT5t7LcO9gge657lH.Vk4BEbxbI1.BtE3EIimrm</t>
+          <t>$2b$10$XtwjjqFCTAXEHgyL25PqNuovXBIU/ktlXS2CBng4MCT.68nA3nPyy</t>
         </is>
       </c>
     </row>
@@ -853,7 +853,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>$2b$10$p50hTk3v2cPELVAW3kDw2OgyEol6y6EPYUlHmJ6qEScwXIHkN35/u</t>
+          <t>$2b$10$OulLiczTAVI3M5J.pdBqUOJA6FBneDmDPthC59Bs1Nhy3xUjzKnwe</t>
         </is>
       </c>
     </row>
@@ -870,7 +870,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>$2b$10$VdDRL..NFjg1jRvxVcbokOBSPpn2lyRU7KiJ0lNJyGAXfOeOYvdbK</t>
+          <t>$2b$10$pDJCcSl9R620anoYhpGG0uWqdin.mUi3py3gFReaQsH/6OkXnRMQC</t>
         </is>
       </c>
     </row>

</xml_diff>